<commit_message>
added upstream mineral data for cement
</commit_message>
<xml_diff>
--- a/data/cement/cement_var.xlsx
+++ b/data/cement/cement_var.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/cement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\cement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602F7481-D8F3-BE4C-A019-0232FCCCB6F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="460" windowWidth="22120" windowHeight="17540" tabRatio="598" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13965" yWindow="465" windowWidth="22125" windowHeight="17535" tabRatio="598" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel" sheetId="28" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="Mixer" sheetId="29" r:id="rId7"/>
     <sheet name="Ref" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>meta-notes</t>
   </si>
@@ -176,15 +175,6 @@
     <t>CaCO3</t>
   </si>
   <si>
-    <t>SiO2</t>
-  </si>
-  <si>
-    <t>AlO2</t>
-  </si>
-  <si>
-    <t>FeO2</t>
-  </si>
-  <si>
     <t>CEMCAP-0C</t>
   </si>
   <si>
@@ -224,12 +214,6 @@
     <t>kg/kg calcined meal</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>MgCO3</t>
-  </si>
-  <si>
     <t>clinker recovery eff</t>
   </si>
   <si>
@@ -260,19 +244,22 @@
     <t>charcoal - IPCC</t>
   </si>
   <si>
-    <t>coal - CEMCAP</t>
-  </si>
-  <si>
     <t>dust in</t>
   </si>
   <si>
     <t>kg/kg meal out</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Marl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -510,8 +497,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -788,30 +775,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F38B04-0302-614C-8C6E-250B6E31288D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FC3BB5-9F80-6647-B0D2-EBF672B93339}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -819,86 +806,54 @@
         <v>30</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0.79300000000000004</v>
       </c>
       <c r="C4">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D4">
-        <v>3.3000000000000002E-2</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="E4">
-        <v>0.02</v>
-      </c>
-      <c r="F4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G4">
-        <f>1-SUM(B4:F4)</f>
-        <v>9.9999999999988987E-4</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="29"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -906,36 +861,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39140EA8-A8E4-7F42-9095-6286906B86F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" style="33"/>
+    <col min="3" max="3" width="10.85546875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -957,21 +912,21 @@
       </c>
       <c r="M1" s="21"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F2" s="25"/>
       <c r="M2" s="21"/>
@@ -980,7 +935,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -990,9 +945,9 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>233098/200025</f>
@@ -1015,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -1024,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1036,33 +991,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621AB658-70D9-5441-BD16-8DE597460781}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1090,22 +1045,22 @@
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
@@ -1119,7 +1074,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1128,9 +1083,9 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>143198/233098</f>
@@ -1150,7 +1105,7 @@
         <v>6.0336038212824204E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1159,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1171,34 +1126,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5BE465-68F2-1C42-8E61-90A64DEA9EBE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="12" max="18" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="12" max="18" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1226,22 +1181,22 @@
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="21"/>
@@ -1255,7 +1210,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1264,9 +1219,9 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>120646/143198</f>
@@ -1286,7 +1241,7 @@
         <v>3.6941856729842598E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1295,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1309,48 +1264,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55113C92-7445-8F47-830C-BF7413622C12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" s="30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1371,54 +1326,54 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A881C3A3-E8FC-0842-9D3C-A892C518175D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0.73699999999999999</v>
@@ -1427,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1439,33 +1394,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
@@ -1474,7 +1429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1441,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1498,7 +1453,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1510,7 +1465,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1522,7 +1477,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1534,7 +1489,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1546,7 +1501,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1559,7 +1514,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -1571,7 +1526,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -1583,24 +1538,24 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="14" t="s">
         <v>20</v>
@@ -1608,7 +1563,7 @@
       <c r="C16" s="14"/>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>21</v>
       </c>
@@ -1617,7 +1572,7 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>22</v>
       </c>
@@ -1629,7 +1584,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>23</v>
       </c>
@@ -1639,7 +1594,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -1649,7 +1604,7 @@
       </c>
       <c r="E20" s="27"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>26</v>
       </c>
@@ -1658,7 +1613,7 @@
         <v>0.90718581887127947</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
standardized beccs cases - pulp and clinker
</commit_message>
<xml_diff>
--- a/data/cement/cement_var.xlsx
+++ b/data/cement/cement_var.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/cement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\cement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BEC2E1-46BB-BE4A-8569-8B6CEE689677}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="460" windowWidth="22120" windowHeight="17540" tabRatio="598" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="465" windowWidth="22125" windowHeight="17535" tabRatio="598" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Meal" sheetId="25" r:id="rId1"/>
     <sheet name="Kiln System" sheetId="32" r:id="rId2"/>
     <sheet name="Cooler" sheetId="31" r:id="rId3"/>
     <sheet name="Mixer" sheetId="29" r:id="rId4"/>
-    <sheet name="Cement Use" sheetId="33" r:id="rId5"/>
-    <sheet name="Ref" sheetId="7" r:id="rId6"/>
-    <sheet name="Preheater" sheetId="30" r:id="rId7"/>
-    <sheet name="Calciner" sheetId="26" r:id="rId8"/>
-    <sheet name="Kiln" sheetId="27" r:id="rId9"/>
+    <sheet name="Ref" sheetId="7" r:id="rId5"/>
+    <sheet name="Preheater" sheetId="30" r:id="rId6"/>
+    <sheet name="Calciner" sheetId="26" r:id="rId7"/>
+    <sheet name="Kiln" sheetId="27" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +75,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="I6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Samantha Eleanor Tanzer - TBM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+included in kiln system</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -106,12 +128,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,12 +204,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,12 +247,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="73">
   <si>
     <t>meta-notes</t>
   </si>
@@ -472,12 +494,18 @@
   </si>
   <si>
     <t>Unspecified Mineral</t>
+  </si>
+  <si>
+    <t>CLK-0B</t>
+  </si>
+  <si>
+    <t>CLK-HB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -765,8 +793,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1043,20 +1071,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1106,7 +1134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1146,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1138,7 +1166,7 @@
       </c>
       <c r="J4" s="29"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1161,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1191,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1218,6 +1246,66 @@
         <v>3.4699999999999953E-2</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="F8">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="G8">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="H8">
+        <f>1-SUM(B8:G8)</f>
+        <v>3.4699999999999953E-2</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="F9">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="G9">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="H9">
+        <f>1-SUM(B9:G9)</f>
+        <v>3.4699999999999953E-2</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
     </row>
@@ -1228,25 +1316,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1370,7 @@
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1311,7 +1399,7 @@
       <c r="S2" s="21"/>
       <c r="T2" s="21"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1342,7 +1430,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1374,7 +1462,7 @@
         <v>0.34920000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1404,7 +1492,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1430,6 +1518,66 @@
         <v>66</v>
       </c>
       <c r="I6">
+        <f>72*Ref!$B$18</f>
+        <v>0.25919999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7">
+        <v>1.53</v>
+      </c>
+      <c r="C7">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3.7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7">
+        <f>72*Ref!$B$18</f>
+        <v>0.25919999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8">
+        <v>1.53</v>
+      </c>
+      <c r="C8">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3.7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8">
         <f>72*Ref!$B$18</f>
         <v>0.25919999999999999</v>
       </c>
@@ -1441,20 +1589,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1471,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1479,12 +1627,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1501,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1518,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1535,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1549,6 +1697,40 @@
         <v>1</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
@@ -1558,16 +1740,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1587,7 +1769,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1604,12 +1786,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1626,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1644,6 +1826,46 @@
       </c>
       <c r="F5">
         <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>0.95</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.05</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>0.95</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.05</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1652,47 +1874,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D858396-432B-814F-8FAD-7B9CEE6CFA13}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
@@ -1701,7 +1909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1713,7 +1921,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1725,7 +1933,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1737,7 +1945,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1749,7 +1957,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1969,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1773,7 +1981,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1786,7 +1994,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +2006,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -1810,24 +2018,24 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="14" t="s">
         <v>20</v>
@@ -1835,7 +2043,7 @@
       <c r="C16" s="14"/>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>21</v>
       </c>
@@ -1844,7 +2052,7 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>22</v>
       </c>
@@ -1856,7 +2064,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>23</v>
       </c>
@@ -1866,7 +2074,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -1876,7 +2084,7 @@
       </c>
       <c r="E20" s="27"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>26</v>
       </c>
@@ -1885,7 +2093,7 @@
         <v>0.90718581887127947</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>29</v>
       </c>
@@ -1896,24 +2104,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="15" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1952,7 +2160,7 @@
       </c>
       <c r="M1" s="21"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1978,7 +2186,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +2196,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2028,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2057,21 +2265,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2113,7 +2321,7 @@
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -2142,7 +2350,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2359,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2193,21 +2401,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="12" max="18" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="12" max="18" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2249,7 +2457,7 @@
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -2278,7 +2486,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2287,7 +2495,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2326,7 +2534,7 @@
       <c r="O4"/>
       <c r="P4"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
electricity sensitivity analysis set up
</commit_message>
<xml_diff>
--- a/data/cement/cement_var.xlsx
+++ b/data/cement/cement_var.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\cement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/cement/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D1641A-D55F-F249-8A8F-A77A642F7433}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="465" windowWidth="22125" windowHeight="17535" tabRatio="598" activeTab="4"/>
+    <workbookView xWindow="6680" yWindow="460" windowWidth="22120" windowHeight="17540" tabRatio="598" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meal" sheetId="25" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Calciner" sheetId="26" r:id="rId7"/>
     <sheet name="Kiln" sheetId="27" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -99,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -128,12 +129,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -204,12 +205,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -247,12 +248,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Eleanor Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -505,7 +506,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -793,8 +794,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1071,20 +1072,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1147,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>0.22999999999999998</v>
       </c>
       <c r="H4">
-        <f>1-SUM(B4:G4)</f>
+        <f t="shared" ref="H4:H9" si="0">1-SUM(B4:G4)</f>
         <v>0</v>
       </c>
       <c r="I4">
@@ -1166,7 +1167,7 @@
       </c>
       <c r="J4" s="29"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1182,14 +1183,14 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <f>1-SUM(B5:G5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1212,14 +1213,14 @@
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="H6">
-        <f>1-SUM(B6:G6)</f>
+        <f t="shared" si="0"/>
         <v>3.4699999999999953E-2</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1242,14 +1243,14 @@
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="H7">
-        <f>1-SUM(B7:G7)</f>
+        <f t="shared" si="0"/>
         <v>3.4699999999999953E-2</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>71</v>
       </c>
@@ -1272,14 +1273,14 @@
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="H8">
-        <f>1-SUM(B8:G8)</f>
+        <f t="shared" si="0"/>
         <v>3.4699999999999953E-2</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>72</v>
       </c>
@@ -1302,7 +1303,7 @@
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="H9">
-        <f>1-SUM(B9:G9)</f>
+        <f t="shared" si="0"/>
         <v>3.4699999999999953E-2</v>
       </c>
       <c r="I9">
@@ -1316,25 +1317,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1370,7 +1371,7 @@
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1400,7 @@
       <c r="S2" s="21"/>
       <c r="T2" s="21"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>0.34920000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>71</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>0.25919999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>72</v>
       </c>
@@ -1589,20 +1590,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1627,12 +1628,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>71</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>72</v>
       </c>
@@ -1740,16 +1741,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -1786,12 +1787,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>71</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>72</v>
       </c>
@@ -1874,33 +1875,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
@@ -1909,7 +1910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>1.963482644775587E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>8.9938431337556905E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>8.0375122691175155E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1994,7 +1995,7 @@
         <v>4.1190030040748338E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -2018,24 +2019,24 @@
         <v>1.4276255911483892E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="14" t="s">
         <v>20</v>
@@ -2043,7 +2044,7 @@
       <c r="C16" s="14"/>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>21</v>
       </c>
@@ -2052,7 +2053,7 @@
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>22</v>
       </c>
@@ -2064,7 +2065,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="27"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>23</v>
       </c>
@@ -2074,7 +2075,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
@@ -2084,7 +2085,7 @@
       </c>
       <c r="E20" s="27"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>26</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>0.90718581887127947</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>29</v>
       </c>
@@ -2105,23 +2106,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="15" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2161,7 @@
       </c>
       <c r="M1" s="21"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -2186,7 +2187,7 @@
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +2197,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2266,20 +2267,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2321,7 +2322,7 @@
       <c r="Q1" s="21"/>
       <c r="R1" s="21"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -2350,7 +2351,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2359,7 +2360,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2402,20 +2403,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="12" max="18" width="10.85546875" style="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="12" max="18" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -2457,7 +2458,7 @@
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>25</v>
       </c>
@@ -2486,7 +2487,7 @@
       <c r="U2" s="21"/>
       <c r="V2" s="21"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2495,7 +2496,7 @@
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2534,7 +2535,7 @@
       <c r="O4"/>
       <c r="P4"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>

</xml_diff>